<commit_message>
ACR implementation guide with updated DocumentReference profile with allintented constraints included, corrected FHIRPAth expressions and updated terminology bindings
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/documentreference-acp-1.xlsx
+++ b/output/AdvanceCareRecords/documentreference-acp-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="393">
   <si>
     <t>Path</t>
   </si>
@@ -146,7 +146,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>A reference to an advance care plan document</t>
+    <t>A reference to an advance care planning document</t>
   </si>
   <si>
     <t>A reference to a document.</t>
@@ -156,7 +156,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-docref-02:If the author is a practitioner, the role shall be provided {(DocumentReference.author.resolve() is Practitioner) implies DocumentReference.extension('http://hl7.org.au/fhir/StructureDefinition/author-role').exists()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-docref-02:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-docref-03:The author shall at least have a reference or an identifier with at least a system and a value {author.reference.exists() or author.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-docref-04:If and only if the author is a practitioner, the role shall be provided {author.resolve().where($this is Practitioner ).exists() implies extension('http://hl7.org.au/fhir/StructureDefinition/author-role').exists()}inv-dh-docref-05:If present, an authoring role shall at least have a reference that conforms to PractitionerRole with Practitioner with Mandatory Identifier or an identifier with at least a system and a value {extension('http://hl7.org.au/fhir/StructureDefinition/author-role').exists() implies extension('http://hl7.org.au/fhir/StructureDefinition/author-role').valueReference.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1') or extension('http://hl7.org.au/fhir/StructureDefinition/author-role').valueReference.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
   </si>
   <si>
     <t>Document[classCode="DOC" and moodCode="EVN"]</t>
@@ -494,7 +494,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-docref-03:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {DocumentReference.extension('http://hl7.org.au/fhir/StructureDefinition/author-role').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>DocumentReference.modifierExtension</t>
@@ -629,7 +629,7 @@
 </t>
   </si>
   <si>
-    <t>Advance Care Planning Document</t>
+    <t>Type of advance care planning document</t>
   </si>
   <si>
     <t>Specifies the particular kind of document referenced  (e.g. History and Physical, Discharge Summary, Progress Note). This usually equates to the purpose of making the document referenced.</t>
@@ -638,21 +638,7 @@
     <t>Key metadata element describing the document, used in searching/filtering.</t>
   </si>
   <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1"/&gt;
-    &lt;code value="100.16998"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
-    <t>preferred</t>
-  </si>
-  <si>
-    <t>Precise type of clinical document.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/c80-doc-typecodes</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/advance-care-planning-document-type-1</t>
   </si>
   <si>
     <t>./code</t>
@@ -701,7 +687,7 @@
     <t>DocumentReference.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -772,11 +758,11 @@
     <t>DocumentReference.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1)
 </t>
   </si>
   <si>
-    <t>Author of the attached advance care plan</t>
+    <t>Author of the attached advance care planning document</t>
   </si>
   <si>
     <t>Identifies who is responsible for adding the information to the document.</t>
@@ -1027,6 +1013,9 @@
   </si>
   <si>
     <t>Note that while IHE mostly issues URNs for format types, not all documents can be identified by a URI.</t>
+  </si>
+  <si>
+    <t>preferred</t>
   </si>
   <si>
     <t>Document Format Codes.</t>
@@ -1425,7 +1414,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.21875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="52.08203125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="82.6875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -3926,31 +3915,29 @@
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W23" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="X23" s="2"/>
+      <c r="Y23" t="s" s="2">
         <v>199</v>
-      </c>
-      <c r="R23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W23" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="X23" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="Y23" t="s" s="2">
-        <v>202</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>40</v>
@@ -3983,25 +3970,25 @@
         <v>40</v>
       </c>
       <c r="AJ23" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AK23" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="AL23" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="AM23" t="s" s="2">
         <v>203</v>
-      </c>
-      <c r="AK23" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="AL23" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="AM23" t="s" s="2">
-        <v>206</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4023,16 +4010,16 @@
         <v>195</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="M24" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="N24" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>40</v>
@@ -4060,57 +4047,57 @@
         <v>109</v>
       </c>
       <c r="X24" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="Y24" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="Z24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE24" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="AF24" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG24" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ24" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="AK24" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="AL24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM24" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="Y24" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="Z24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE24" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="AF24" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG24" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ24" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="AK24" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="AL24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM24" t="s" s="2">
-        <v>216</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4133,13 +4120,13 @@
         <v>51</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -4190,7 +4177,7 @@
         <v>40</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>41</v>
@@ -4205,21 +4192,21 @@
         <v>40</v>
       </c>
       <c r="AJ25" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="AK25" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AM25" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="AK25" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="AL25" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="AM25" t="s" s="2">
-        <v>224</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4242,16 +4229,16 @@
         <v>51</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="M26" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="K26" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>229</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -4301,7 +4288,7 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
@@ -4316,21 +4303,21 @@
         <v>40</v>
       </c>
       <c r="AJ26" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AK26" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="AL26" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="AM26" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="AK26" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="AL26" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="AM26" t="s" s="2">
-        <v>233</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4356,13 +4343,13 @@
         <v>85</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4412,7 +4399,7 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>50</v>
@@ -4427,21 +4414,21 @@
         <v>40</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4464,16 +4451,16 @@
         <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="K28" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="L28" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="M28" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="K28" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4523,7 +4510,7 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>41</v>
@@ -4538,21 +4525,21 @@
         <v>40</v>
       </c>
       <c r="AJ28" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="AK28" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="AL28" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="AM28" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="AK28" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="AL28" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="AM28" t="s" s="2">
-        <v>248</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4575,16 +4562,16 @@
         <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="M29" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="K29" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4634,7 +4621,7 @@
         <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -4649,21 +4636,21 @@
         <v>40</v>
       </c>
       <c r="AJ29" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="AM29" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="AM29" t="s" s="2">
-        <v>257</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4686,16 +4673,16 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="K30" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="M30" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="K30" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>262</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -4745,7 +4732,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4760,7 +4747,7 @@
         <v>40</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>40</v>
@@ -4774,7 +4761,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4797,16 +4784,16 @@
         <v>51</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="K31" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="M31" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="K31" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>268</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4856,7 +4843,7 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>41</v>
@@ -4868,10 +4855,10 @@
         <v>40</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>40</v>
@@ -4885,7 +4872,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4994,7 +4981,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5105,11 +5092,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5134,7 +5121,7 @@
         <v>154</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>74</v>
@@ -5187,7 +5174,7 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5216,7 +5203,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5242,13 +5229,13 @@
         <v>119</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
@@ -5277,57 +5264,57 @@
         <v>178</v>
       </c>
       <c r="X35" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="Y35" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE35" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="Y35" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="Z35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AF35" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>284</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5350,13 +5337,13 @@
         <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5407,7 +5394,7 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>50</v>
@@ -5422,7 +5409,7 @@
         <v>40</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>40</v>
@@ -5431,12 +5418,12 @@
         <v>40</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5462,16 +5449,16 @@
         <v>64</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="N37" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>295</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>40</v>
@@ -5520,7 +5507,7 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5535,21 +5522,21 @@
         <v>40</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5575,16 +5562,16 @@
         <v>195</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="N38" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5633,7 +5620,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5648,21 +5635,21 @@
         <v>40</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5685,13 +5672,13 @@
         <v>51</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5742,7 +5729,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>50</v>
@@ -5754,10 +5741,10 @@
         <v>40</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>40</v>
@@ -5771,7 +5758,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5880,7 +5867,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5991,11 +5978,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6020,7 +6007,7 @@
         <v>154</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>74</v>
@@ -6073,7 +6060,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -6102,7 +6089,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6125,13 +6112,13 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6182,7 +6169,7 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>50</v>
@@ -6197,21 +6184,21 @@
         <v>40</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6237,13 +6224,13 @@
         <v>97</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6269,60 +6256,60 @@
         <v>40</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>200</v>
+        <v>321</v>
       </c>
       <c r="X44" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM44" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="Y44" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="Z44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="AF44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG44" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ44" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="AK44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM44" t="s" s="2">
-        <v>326</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6345,16 +6332,16 @@
         <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="M45" t="s" s="2">
         <v>328</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
@@ -6404,7 +6391,7 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6416,10 +6403,10 @@
         <v>40</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>40</v>
@@ -6433,7 +6420,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6542,7 +6529,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6653,11 +6640,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6682,7 +6669,7 @@
         <v>154</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>74</v>
@@ -6735,7 +6722,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6764,7 +6751,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6787,13 +6774,13 @@
         <v>51</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="K49" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6844,7 +6831,7 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
@@ -6859,10 +6846,10 @@
         <v>40</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>40</v>
@@ -6873,7 +6860,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6899,13 +6886,13 @@
         <v>195</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -6934,10 +6921,10 @@
         <v>109</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>40</v>
@@ -6955,7 +6942,7 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -6970,7 +6957,7 @@
         <v>40</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>40</v>
@@ -6979,12 +6966,12 @@
         <v>40</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7007,13 +6994,13 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7064,7 +7051,7 @@
         <v>40</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7079,7 +7066,7 @@
         <v>40</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>40</v>
@@ -7088,12 +7075,12 @@
         <v>40</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7119,10 +7106,10 @@
         <v>195</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7152,57 +7139,57 @@
         <v>109</v>
       </c>
       <c r="X52" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="Y52" t="s" s="2">
+      <c r="AK52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG52" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>361</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7228,16 +7215,16 @@
         <v>195</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>363</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="N53" t="s" s="2">
         <v>364</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>366</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>40</v>
@@ -7265,57 +7252,57 @@
         <v>109</v>
       </c>
       <c r="X53" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM53" t="s" s="2">
         <v>367</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="AF53" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG53" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>369</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7338,13 +7325,13 @@
         <v>51</v>
       </c>
       <c r="J54" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7395,7 +7382,7 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7410,7 +7397,7 @@
         <v>40</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>40</v>
@@ -7419,12 +7406,12 @@
         <v>40</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7447,16 +7434,16 @@
         <v>51</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
@@ -7506,7 +7493,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7518,10 +7505,10 @@
         <v>40</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>40</v>
@@ -7530,12 +7517,12 @@
         <v>40</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7644,7 +7631,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7755,11 +7742,11 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -7784,7 +7771,7 @@
         <v>154</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="M58" t="s" s="2">
         <v>74</v>
@@ -7837,7 +7824,7 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7866,7 +7853,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7892,13 +7879,13 @@
         <v>158</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -7948,7 +7935,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -7963,7 +7950,7 @@
         <v>40</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>40</v>
@@ -7977,7 +7964,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8000,16 +7987,16 @@
         <v>51</v>
       </c>
       <c r="J60" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="K60" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="K60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>392</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
@@ -8059,7 +8046,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8074,7 +8061,7 @@
         <v>40</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>40</v>

</xml_diff>